<commit_message>
task 1 noteboo update with few shot
</commit_message>
<xml_diff>
--- a/data/output/classified_messages.xlsx
+++ b/data/output/classified_messages.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>Gampaha</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -572,7 +572,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -589,7 +589,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -606,7 +606,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -657,7 +657,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -674,7 +674,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kolonnawa</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -742,7 +742,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -793,7 +793,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Kaduwela</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -810,7 +810,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -827,7 +827,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -929,7 +929,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Galle</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -973,19 +973,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Info</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -997,12 +997,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Supply</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1082,7 +1082,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1116,12 +1116,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Supply</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1138,36 +1138,36 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Supply</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Rescue</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1184,7 +1184,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Matale</t>
+          <t>Kandy</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1218,12 +1218,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Info</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1235,7 +1235,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1269,12 +1269,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Info</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1286,12 +1286,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>[None]</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Info</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">

</xml_diff>